<commit_message>
Obj,Fbx 업로드 & Obj.xlsx 업데이트
</commit_message>
<xml_diff>
--- a/Documents/Obj.xlsx
+++ b/Documents/Obj.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03ad4a8e8f7310f3/기획/졸업작품/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03ad4a8e8f7310f3/project/GangsterHamster/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE73DCE-E47C-462A-A3DA-25112E068CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{5BE73DCE-E47C-462A-A3DA-25112E068CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{712B985F-0A60-491E-A197-DD9466A3E811}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="3780" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -278,6 +278,28 @@
 버튼이 있으며, 천장에는
 침대를 비추는, 사각형의
 큰 조명이 있으면 좋겠어요. 그리고, 추가로 여러 모니터 같은 게 붙어 있으면 더 좋을 거 같아요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰색 점토로 만들어진 듯 한 벽에
+금이 있어, 일정 이상의 힘을 가하면
+부서질 것만 같은 벽이 필요합니다.
+또한 일정 이상의 힘이 가해진다면
+벽이 여러 조각으로 분해되어
+바닥을 나뒹굴어야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">양쪽으로 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>움직이는 발판이 존재하며, 버튼과 연계된 발판의 경우 
+버튼 활성화 시 3초에 걸쳐 목적 위치까지 도달함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1m x </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,7 +547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -603,6 +625,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -755,15 +783,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>33616</xdr:colOff>
+      <xdr:colOff>302558</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:rowOff>246529</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2113427</xdr:colOff>
+      <xdr:colOff>2382369</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2256658</xdr:rowOff>
+      <xdr:rowOff>2323893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -793,7 +821,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9491381" y="9502588"/>
+          <a:off x="15273617" y="952500"/>
           <a:ext cx="2079811" cy="2077364"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -816,13 +844,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2324101</xdr:colOff>
+      <xdr:colOff>2559424</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>168091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>4869515</xdr:colOff>
+      <xdr:colOff>5104838</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>2244845</xdr:rowOff>
     </xdr:to>
@@ -854,7 +882,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11781866" y="9491385"/>
+          <a:off x="17530483" y="874062"/>
           <a:ext cx="2545414" cy="2076754"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1415,6 +1443,555 @@
         <a:xfrm>
           <a:off x="19920857" y="15441530"/>
           <a:ext cx="4313464" cy="2434519"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>204107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3324225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>5042807</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="그림 16" descr="우주 정거장 내부 화장실 방입니다 우주선에 변기와 빈 화장실 우주 비행사에 대 한 공간 화장실입니다 Mir Space Station에  대한 스톡 사진 및 기타 이미지 - iStock">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558B1A8E-0CB5-4C23-859C-075342765928}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15090321" y="12164786"/>
+          <a:ext cx="3228975" cy="4838700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3633108</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>340177</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9189348</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4905373</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="그림 17" descr="우주에서의 배설물은 어떻게 처리할까? : 네이버 블로그">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0AB486B-BE3F-49AB-9FE7-F85277FFE8FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="18628179" y="12300856"/>
+          <a:ext cx="5556240" cy="4565196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1292806</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4708071</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4342463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="그림 19" descr="배경으로 오래된 흙 벽 로열티 무료 사진, 그림, 이미지 그리고 스톡포토그래피. Image 22856987.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73A7DD75-518A-4A20-AFAF-CD081FD10A91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15158357" y="26411592"/>
+          <a:ext cx="4544785" cy="3049657"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4857749</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8844643</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2402839</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="그림 20" descr="흙벽예찬 흙집 황토흙 황토벽 만들기 : 네이버 블로그">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83B1CAEC-6916-4667-B6B7-6D5CA8F07C50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19852820" y="25214036"/>
+          <a:ext cx="3986894" cy="2307589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5034644</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>2585354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8668208</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5143499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="그림 21" descr="한 무더기의 부서진 돌 | 돌, 질감, 부서진">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B1CBA65-424B-48B0-9F15-CAACFBE26FD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="20029715" y="27704140"/>
+          <a:ext cx="3633564" cy="2558145"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>432956</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4087091</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>5066645</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="그림 22" descr="열린목공방 - 철제느낌 원목 캐비넷-(열린목공방,강서구목공방,가구공방,diy가구교실,가구만들기)">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3368749B-661D-45C6-81F2-252344E62813}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15430501" y="10338954"/>
+          <a:ext cx="3654135" cy="4893464"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>301831</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>253587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6982938</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5056909</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="그림 23" descr="에뛰드 하우스 :: 민트 캐비닛">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8132CFD6-9467-4DBC-BF74-C35A7E0B92AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15299376" y="8566314"/>
+          <a:ext cx="6681107" cy="4803322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>557894</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>368558</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3728358</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3562349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="그림 25" descr="무빙 워크 및 에스컬레이터 컬렉션 3D 모델 $49 - .max .obj .fbx .3ds - Free3D">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8878A084-ABD0-4CA7-9562-B6724F38AD4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15552965" y="29855237"/>
+          <a:ext cx="3170464" cy="3193791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4558394</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>517071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8811987</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3374571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="그림 26" descr="무빙워크 사진, 이미지, 일러스트, 캘리그라피 - 크라우드픽">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE7FDFD3-4B04-4094-9D31-A021B6898347}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19553465" y="30003750"/>
+          <a:ext cx="4253593" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1831,7 +2408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.3"/>
@@ -1890,7 +2467,9 @@
       <c r="F2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1915,7 +2494,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="145.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="408.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1927,11 +2506,12 @@
         <v>15</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1947,7 +2527,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1993,8 +2573,9 @@
       <c r="E8" s="4"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
+      <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="304.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -2090,7 +2671,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="189.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -2103,6 +2684,9 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="9"/>
+      <c r="G15" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
@@ -2162,8 +2746,8 @@
       <c r="D18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>19</v>
+      <c r="E18" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>43</v>

</xml_diff>